<commit_message>
Fixed the names of the analyses
</commit_message>
<xml_diff>
--- a/projects/DC_analysis/PTool_5_of_5.xlsx
+++ b/projects/DC_analysis/PTool_5_of_5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="-12" yWindow="3000" windowWidth="10296" windowHeight="2364" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -1343,9 +1343,6 @@
     <t>1.14.7</t>
   </si>
   <si>
-    <t>Ptool_4_of_5</t>
-  </si>
-  <si>
     <t>cluster4</t>
   </si>
   <si>
@@ -1479,6 +1476,9 @@
   </si>
   <si>
     <t>Run Measure exterior lighting control</t>
+  </si>
+  <si>
+    <t>Ptool_5_of_5</t>
   </si>
 </sst>
 </file>
@@ -4003,13 +4003,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1842">
     <cellStyle name="20% - Accent1" xfId="1819" builtinId="30" customBuiltin="1"/>
@@ -6188,8 +6188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6258,7 +6258,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>100</v>
@@ -6329,7 +6329,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>435</v>
+        <v>480</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>99</v>
@@ -6681,14 +6681,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -6913,7 +6913,7 @@
         <v>374</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>375</v>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="C9" s="49"/>
       <c r="D9" s="49" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E9" s="49" t="s">
         <v>262</v>
@@ -6999,7 +6999,7 @@
         <v>378</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>379</v>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="49" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E12" s="49" t="s">
         <v>262</v>
@@ -7060,7 +7060,7 @@
         <v>380</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>381</v>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="49" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E14" s="49" t="s">
         <v>262</v>
@@ -7121,7 +7121,7 @@
         <v>382</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>383</v>
@@ -7138,7 +7138,7 @@
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="49" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E16" s="49" t="s">
         <v>262</v>
@@ -7182,7 +7182,7 @@
         <v>384</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>385</v>
@@ -7199,7 +7199,7 @@
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="49" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E18" s="49" t="s">
         <v>262</v>
@@ -7316,7 +7316,7 @@
         <v>392</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>393</v>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E23" s="49" t="s">
         <v>262</v>
@@ -7402,7 +7402,7 @@
         <v>395</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D25" s="35" t="s">
         <v>396</v>
@@ -7419,7 +7419,7 @@
       </c>
       <c r="C26" s="49"/>
       <c r="D26" s="49" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E26" s="49" t="s">
         <v>262</v>
@@ -7463,7 +7463,7 @@
         <v>397</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>398</v>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="49" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E28" s="49" t="s">
         <v>262</v>
@@ -7524,7 +7524,7 @@
         <v>427</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D29" s="35" t="s">
         <v>428</v>
@@ -7541,7 +7541,7 @@
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E30" s="49" t="s">
         <v>262</v>
@@ -7585,7 +7585,7 @@
         <v>429</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D31" s="35" t="s">
         <v>430</v>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E32" s="49" t="s">
         <v>262</v>
@@ -7663,58 +7663,58 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="51" t="s">
+    <row r="34" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="50" t="s">
         <v>339</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="50" t="s">
+        <v>478</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="52"/>
+    </row>
+    <row r="35" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="50" t="s">
         <v>479</v>
       </c>
-      <c r="D34" s="51" t="s">
-        <v>340</v>
-      </c>
-      <c r="E34" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" s="53"/>
-    </row>
-    <row r="35" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="51" t="s">
-        <v>480</v>
-      </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="50" t="s">
         <v>262</v>
       </c>
-      <c r="G35" s="51" t="s">
+      <c r="G35" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="51">
-        <v>1</v>
-      </c>
-      <c r="J35" s="53"/>
-      <c r="K35" s="54">
+      <c r="I35" s="50">
+        <v>1</v>
+      </c>
+      <c r="J35" s="52"/>
+      <c r="K35" s="53">
         <v>0</v>
       </c>
-      <c r="L35" s="54">
-        <v>1</v>
-      </c>
-      <c r="M35" s="54">
-        <v>1</v>
-      </c>
-      <c r="N35" s="54">
-        <v>1</v>
-      </c>
-      <c r="O35" s="54"/>
-      <c r="P35" s="54" t="s">
+      <c r="L35" s="53">
+        <v>1</v>
+      </c>
+      <c r="M35" s="53">
+        <v>1</v>
+      </c>
+      <c r="N35" s="53">
+        <v>1</v>
+      </c>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="R35" s="51" t="s">
+      <c r="R35" s="50" t="s">
         <v>259</v>
       </c>
     </row>
@@ -7732,7 +7732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
@@ -8375,13 +8375,13 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F22" s="47" t="s">
         <v>43</v>
@@ -8398,13 +8398,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F23" s="47" t="s">
         <v>43</v>
@@ -8421,13 +8421,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F24" s="47" t="s">
         <v>43</v>
@@ -8444,13 +8444,13 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>43</v>
@@ -8467,13 +8467,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F26" s="47" t="s">
         <v>43</v>
@@ -8490,13 +8490,13 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>43</v>
@@ -8513,13 +8513,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>43</v>
@@ -8536,13 +8536,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>43</v>
@@ -8559,13 +8559,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>43</v>
@@ -8582,13 +8582,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>43</v>
@@ -8604,27 +8604,27 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="50" t="s">
+        <v>476</v>
+      </c>
+      <c r="B32" s="50" t="s">
+        <v>476</v>
+      </c>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="B32" s="51" t="s">
-        <v>477</v>
-      </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51" t="s">
-        <v>478</v>
-      </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52" t="s">
+      <c r="E32" s="50"/>
+      <c r="F32" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="52" t="b">
+      <c r="G32" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="51" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>